<commit_message>
modified:   Extractor/Sample.py 	modified:   Extractor/VariablesWindow.py 	modified:   test/Tensile_test.xlsx
</commit_message>
<xml_diff>
--- a/test/Tensile_test.xlsx
+++ b/test/Tensile_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quentin.raball\Documents\Python\tensile_test_analyzer\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CEF33A-EE23-4041-BE95-B5B4B1F6E884}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9150F4C7-2EDB-492A-AC7C-51726D7B9352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
   <si>
     <t>N° test</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Chaque échantillon contenu dans le même fichier dispose de sa propre ligne.</t>
   </si>
   <si>
-    <t>Le programme s'exécute sans erreur et la fenêtre principale s'ouvre.</t>
-  </si>
-  <si>
     <t>Ajout d'un fichier supplémentaire</t>
   </si>
   <si>
@@ -253,9 +250,6 @@
   </si>
   <si>
     <t>Analyse traction</t>
-  </si>
-  <si>
-    <t>Analyse Flexion</t>
   </si>
   <si>
     <t>Configurer l'échantillon C35 comme cela : 
@@ -338,6 +332,61 @@
 Defo = 0.647 % 
 E = 291 GPa</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Le programme s'exécute sans erreur et la fenêtre principale s'ouvre. Si un fichier est présent mais n'est pas reconnu comme valide, le programme </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>crash</t>
+    </r>
+  </si>
+  <si>
+    <t>Analyse Flexion 3 pts</t>
+  </si>
+  <si>
+    <t>Analyse Flexion 4 pts</t>
+  </si>
+  <si>
+    <r>
+      <t>./Data/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Exemple_Shimadzu_Flex4_L20_D2.csv</t>
+    </r>
+  </si>
+  <si>
+    <t>Configurer l'échantillon Flex4 comme cela : 
+Mesure traverse (Shimadzu)
+Mode d'analyse: Flexion 4pts
+Géométrie: Ronde
+D0 = 2
+L0 = 20
+F_Max = 300
+F_Min = 150</t>
+  </si>
+  <si>
+    <t>Résultats Correctes (Interface Shimadzu): A OBTENIR
+F_Max =  N
+Allong = mm
+Re = MPa
+Rm =  Mpa
+Defo =  % 
+E =  GPa</t>
   </si>
 </sst>
 </file>
@@ -388,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -405,6 +454,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -688,27 +740,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="43.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="32.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="46.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="32.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>1</v>
@@ -717,7 +769,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>2</v>
@@ -729,12 +781,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -743,13 +795,13 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -761,13 +813,13 @@
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -779,335 +831,350 @@
         <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="F16" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
       <c r="B23" s="6"/>
+      <c r="C23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>81</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Ajout menu changement theme
</commit_message>
<xml_diff>
--- a/test/Tensile_test.xlsx
+++ b/test/Tensile_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quentin.raball\Documents\Python\tensile_test_analyzer\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9150F4C7-2EDB-492A-AC7C-51726D7B9352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B533FC-FF4A-4D69-9CB0-DD7FD794D4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="85">
   <si>
     <t>N° test</t>
   </si>
@@ -387,6 +387,23 @@
 Rm =  Mpa
 Defo =  % 
 E =  GPa</t>
+  </si>
+  <si>
+    <t>Analyse Module de Young</t>
+  </si>
+  <si>
+    <t>./Data/Exemple_WB100kN_Young</t>
+  </si>
+  <si>
+    <t>Configurer l'échantillon comme cela : 
+Mesure extenso (W+B 100kN)
+Mode d'analyse: Flexion 4pts
+Géométrie: Ronde
+D0 = 2
+L0 = 50
+L1= 20
+F_Max = 300
+F_Min = 150</t>
   </si>
 </sst>
 </file>
@@ -738,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1120,7 +1137,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1176,12 +1193,30 @@
         <v>81</v>
       </c>
     </row>
+    <row r="24" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B21:B23"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B5:B13"/>
     <mergeCell ref="B14:B20"/>
+    <mergeCell ref="B21:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Amélioration fenêtre post-analyse - Gestion des options
</commit_message>
<xml_diff>
--- a/test/Tensile_test.xlsx
+++ b/test/Tensile_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quentin.raball\Documents\Python\tensile_test_analyzer\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B533FC-FF4A-4D69-9CB0-DD7FD794D4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C194A048-9C91-440E-AE91-EFB98DB84EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="95">
   <si>
     <t>N° test</t>
   </si>
@@ -404,6 +404,36 @@
 L1= 20
 F_Max = 300
 F_Min = 150</t>
+  </si>
+  <si>
+    <t>Importation de fichiers faux</t>
+  </si>
+  <si>
+    <t>./Data/Erreur.csv</t>
+  </si>
+  <si>
+    <t>Le programme analyse le dossier "Data", le fichier posant problème est skippé. Un message d'avertissement apparait pour avertir l'utilisateur.</t>
+  </si>
+  <si>
+    <t>Titres des graphiques exportés</t>
+  </si>
+  <si>
+    <t>Legendes graphiques exportés</t>
+  </si>
+  <si>
+    <t>Cocher les cases "Nom du sample" et "Nom du fichier". Configurer le sample. Analyser le sample. Exporter tous les graphiques individuels.</t>
+  </si>
+  <si>
+    <t>Comportement de l'exportation</t>
+  </si>
+  <si>
+    <t>Cocher la case "Légendes". Configurer et analyser le sample. Exporter tous les graphiques individuels.</t>
+  </si>
+  <si>
+    <t>Le graphique "Contrainte - Déformation" ne doit plus contenir la légende. Les graphiques post-analyses n'ont plus de légende non-plus</t>
+  </si>
+  <si>
+    <t>Chaque graphique exporté dispose du nom de sample ainsi que le nom du fichier. Si les cases sont décochées, les graphiques n'ont pas de nom. Les graphiques post-analyses ont la légende qui dépend directement de ces cases.</t>
   </si>
 </sst>
 </file>
@@ -454,13 +484,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -469,17 +496,55 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -490,6 +555,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AE5D4152-04EF-4CF7-8FFE-99605E0D0423}" name="Tableau1" displayName="Tableau1" ref="A1:H1048576" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
+  <autoFilter ref="A1:H1048576" xr:uid="{AE5D4152-04EF-4CF7-8FFE-99605E0D0423}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{C07BC986-3EF1-4276-97AE-ED6DE5B925B1}" name="N° test"/>
+    <tableColumn id="2" xr3:uid="{02BCC165-8B77-442B-9E0B-9B8E9DD10767}" name="Elements concernés" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{75B78F65-CE37-4359-A14D-6A817DDC40E6}" name="Tâche à accomplir" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{5B390D10-DC6D-49AB-B39D-B4CBB87B2B93}" name="Elements utiles"/>
+    <tableColumn id="5" xr3:uid="{51143154-2385-4055-BC76-4784A6A49AD4}" name="Etapes réalisées" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{2FC068A9-E8F1-4B24-81A3-AE91BC18AE0A}" name="Résultat théorique" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{EC596E49-3D6B-4282-8830-A46007A133E6}" name="Résultat obtenu" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{315F5128-D998-4EE4-8AFB-7ABCDF945028}" name="Fail/pass"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -755,15 +837,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="6" customWidth="1"/>
     <col min="3" max="3" width="24.5546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="44.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.33203125" style="1" customWidth="1"/>
@@ -772,33 +855,33 @@
     <col min="8" max="8" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -822,7 +905,9 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
@@ -840,7 +925,9 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
@@ -854,371 +941,491 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="6"/>
+      <c r="B13" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="C15" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="C16" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="C17" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="6"/>
+      <c r="B18" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="C18" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="6"/>
+      <c r="B19" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="C19" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="6"/>
+      <c r="B20" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="C20" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="6"/>
+      <c r="B22" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="C22" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="6"/>
+      <c r="B23" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="C23" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D23" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="6"/>
+      <c r="B24" s="6" t="s">
+        <v>70</v>
+      </c>
       <c r="C24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>83</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F25" s="5" t="s">
         <v>81</v>
       </c>
     </row>
+    <row r="26" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B31" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B13"/>
-    <mergeCell ref="B14:B20"/>
-    <mergeCell ref="B21:B24"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correction bug tables lors de l'exportation des graphiques
</commit_message>
<xml_diff>
--- a/test/Tensile_test.xlsx
+++ b/test/Tensile_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quentin.raball\Documents\Python\tensile_test_analyzer\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C194A048-9C91-440E-AE91-EFB98DB84EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AEBA481-3AB2-40DF-B009-F71E264FC6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="110">
   <si>
     <t>N° test</t>
   </si>
@@ -434,6 +434,64 @@
   </si>
   <si>
     <t>Chaque graphique exporté dispose du nom de sample ainsi que le nom du fichier. Si les cases sont décochées, les graphiques n'ont pas de nom. Les graphiques post-analyses ont la légende qui dépend directement de ces cases.</t>
+  </si>
+  <si>
+    <t>Déformation affichée en %</t>
+  </si>
+  <si>
+    <t>Cocher la case "Déformation en %". Configurer et analyser le sample. Exporter tous les graphiques individuels</t>
+  </si>
+  <si>
+    <t>L'axe de "Déformation" dans le graphique "Contrainte - Déformation" doit être en [%], le rp02 passant par la valeur 0.2 %. Si la case est décochée, tout doit être divisé d'un facteur 100 et rp02 doit passer par la valeur 0.002</t>
+  </si>
+  <si>
+    <t>Analyse traction avec extensomètre</t>
+  </si>
+  <si>
+    <t>Configurer l'échantillon comme cela : 
+Mesure Extensomètre (W+B 100kN)
+Mode d'analyse: Traction
+Géométrie : Ronde
+D0 = 2
+L0 = 100
+F_Max = 4000
+F_Min = 2000</t>
+  </si>
+  <si>
+    <t>Résultats Correctes (DataExtractorV10):
+F_Max = 8340 N
+Allong = 18.3 mm (A controler)
+Re = 2010 MPa
+Rm = 2660 Mpa
+Defo = 17.3 % 
+E = 169 GPa</t>
+  </si>
+  <si>
+    <t>Affichage de la droite élastique</t>
+  </si>
+  <si>
+    <t>Le graphique "Contrainte - Déformation" ne doit plus contenir la droite de limite élastique.</t>
+  </si>
+  <si>
+    <t>Affichages des tables dans les graphiques</t>
+  </si>
+  <si>
+    <t>Cocher la case "Droite limite élastique". Configurer et analyser le sample. Exporter tous les graphiques individuels</t>
+  </si>
+  <si>
+    <t>Cocher la case "Montrer résultats calculés". Configurer et analyser le sample. Exporter les graphiques individuels.</t>
+  </si>
+  <si>
+    <t>Les graphiques doivent avoir la table affichées avec les valeurs max du graphiques. Les noms et unités dépendent du type de graphique et sont adaptés au cas par cas.</t>
+  </si>
+  <si>
+    <t>Forcer l'affichage des valeurs de forces en [kN]</t>
+  </si>
+  <si>
+    <t>Cocher la case "Utilisation des {kN}". Configurer et analyser le sample. Exporter les graphiques individuels.</t>
+  </si>
+  <si>
+    <t>Les graphiques "Forces" doivent avoir l'axe adapté d'un facteur 1000. Les tables doivent aussi avoir la valeur adaptée.</t>
   </si>
 </sst>
 </file>
@@ -837,10 +895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1300,16 +1358,16 @@
         <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>75</v>
+        <v>99</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
@@ -1320,19 +1378,19 @@
         <v>70</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1340,39 +1398,39 @@
         <v>70</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D25" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1380,45 +1438,116 @@
         <v>91</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C29" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C30" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
       <c r="B31" s="6" t="s">
         <v>91</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout des derniers tests a effectuer. Rouge pour vérification
</commit_message>
<xml_diff>
--- a/test/Tensile_test.xlsx
+++ b/test/Tensile_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quentin.raball\Documents\Python\tensile_test_analyzer\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AEBA481-3AB2-40DF-B009-F71E264FC6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437B2C5A-F144-4CBF-B36F-7AA4DDC34C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="117">
   <si>
     <t>N° test</t>
   </si>
@@ -492,6 +492,27 @@
   </si>
   <si>
     <t>Les graphiques "Forces" doivent avoir l'axe adapté d'un facteur 1000. Les tables doivent aussi avoir la valeur adaptée.</t>
+  </si>
+  <si>
+    <t>Comportement des option d'analyse</t>
+  </si>
+  <si>
+    <t>Changement des chiffres significatifs</t>
+  </si>
+  <si>
+    <t>Passer l'option des chiffres significatifs sur 5. Configurer et analyser le sample. Exporter les graphiques individuels. Ouvrir la fenêtre des variables.</t>
+  </si>
+  <si>
+    <t>Les chiffres significatifs devraient être de 5 partout où cela est possible: Les tables des graphiques exportés; Fenêtre des variables; Fenêtre post-analyse et tableaux exportés (VarWin &amp; PAWin).</t>
+  </si>
+  <si>
+    <t>Changement dedéfinition limite élastique</t>
+  </si>
+  <si>
+    <t>Passer l'option de Définition de limite élastique à 0.5% pour optenir Rp0.5 par la suite. Configurer et analyser le sample. Exporter les graphiques individuels.</t>
+  </si>
+  <si>
+    <t>La définition de Re passe à 0.5%. Les résultats calculés pour Re doivent avoir été adaptés en conséquence. Vérifier sur les graphique "Contrainte - Déformation" que la droite change bien de position.</t>
   </si>
 </sst>
 </file>
@@ -895,10 +916,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1015,7 +1036,7 @@
       <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="5" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1548,6 +1569,46 @@
       </c>
       <c r="F32" s="1" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new file:   Data/Exemple_Erreur_Import_Largeur_Incorrecte.csv 	modified:   test/Tensile_test.xlsx
</commit_message>
<xml_diff>
--- a/test/Tensile_test.xlsx
+++ b/test/Tensile_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quentin.raball\Documents\Python\tensile_test_analyzer\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437B2C5A-F144-4CBF-B36F-7AA4DDC34C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677ABE89-83E3-44A4-8F57-3F8BCC56B4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="121">
   <si>
     <t>N° test</t>
   </si>
@@ -334,21 +334,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Le programme s'exécute sans erreur et la fenêtre principale s'ouvre. Si un fichier est présent mais n'est pas reconnu comme valide, le programme </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>crash</t>
-    </r>
-  </si>
-  <si>
     <t>Analyse Flexion 3 pts</t>
   </si>
   <si>
@@ -513,6 +498,21 @@
   </si>
   <si>
     <t>La définition de Re passe à 0.5%. Les résultats calculés pour Re doivent avoir été adaptés en conséquence. Vérifier sur les graphique "Contrainte - Déformation" que la droite change bien de position.</t>
+  </si>
+  <si>
+    <t>Le programme s'exécute sans erreur et la fenêtre principale s'ouvre. Si un fichier est présent mais n'est pas reconnu comme valide, le programme le skip</t>
+  </si>
+  <si>
+    <t>Le programme s'exécute correctement</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Le programme détecte les fichiers correctement et les listes correctement</t>
+  </si>
+  <si>
+    <t>Le programme détecte les fichiers multiples correctement. Chaque sample est disposé sur une ligne</t>
   </si>
 </sst>
 </file>
@@ -587,6 +587,18 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -611,18 +623,6 @@
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -637,16 +637,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AE5D4152-04EF-4CF7-8FFE-99605E0D0423}" name="Tableau1" displayName="Tableau1" ref="A1:H1048576" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AE5D4152-04EF-4CF7-8FFE-99605E0D0423}" name="Tableau1" displayName="Tableau1" ref="A1:H1048576" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:H1048576" xr:uid="{AE5D4152-04EF-4CF7-8FFE-99605E0D0423}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{C07BC986-3EF1-4276-97AE-ED6DE5B925B1}" name="N° test"/>
-    <tableColumn id="2" xr3:uid="{02BCC165-8B77-442B-9E0B-9B8E9DD10767}" name="Elements concernés" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{75B78F65-CE37-4359-A14D-6A817DDC40E6}" name="Tâche à accomplir" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{02BCC165-8B77-442B-9E0B-9B8E9DD10767}" name="Elements concernés" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{75B78F65-CE37-4359-A14D-6A817DDC40E6}" name="Tâche à accomplir" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{5B390D10-DC6D-49AB-B39D-B4CBB87B2B93}" name="Elements utiles"/>
-    <tableColumn id="5" xr3:uid="{51143154-2385-4055-BC76-4784A6A49AD4}" name="Etapes réalisées" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{2FC068A9-E8F1-4B24-81A3-AE91BC18AE0A}" name="Résultat théorique" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{EC596E49-3D6B-4282-8830-A46007A133E6}" name="Résultat obtenu" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{51143154-2385-4055-BC76-4784A6A49AD4}" name="Etapes réalisées" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{2FC068A9-E8F1-4B24-81A3-AE91BC18AE0A}" name="Résultat théorique" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{EC596E49-3D6B-4282-8830-A46007A133E6}" name="Résultat obtenu" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{315F5128-D998-4EE4-8AFB-7ABCDF945028}" name="Fail/pass"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -918,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -977,7 +977,13 @@
         <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>76</v>
+        <v>116</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -999,8 +1005,14 @@
       <c r="F3" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1018,6 +1030,12 @@
       </c>
       <c r="F4" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H4" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1028,16 +1046,16 @@
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" t="s">
         <v>85</v>
-      </c>
-      <c r="D5" t="s">
-        <v>86</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1379,16 +1397,16 @@
         <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D23" t="s">
         <v>56</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
@@ -1399,7 +1417,7 @@
         <v>70</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
@@ -1419,16 +1437,16 @@
         <v>70</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" t="s">
         <v>78</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -1439,16 +1457,16 @@
         <v>70</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" t="s">
         <v>82</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="F26" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -1456,19 +1474,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1476,19 +1494,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -1496,19 +1514,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1516,19 +1534,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="D30" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -1536,19 +1554,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D31" t="s">
         <v>10</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -1556,19 +1574,19 @@
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D32" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -1576,19 +1594,19 @@
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D33" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -1596,19 +1614,19 @@
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D34" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correction problèmes diverses. Beta 1.2
</commit_message>
<xml_diff>
--- a/test/Tensile_test.xlsx
+++ b/test/Tensile_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quentin.raball\Documents\Python\tensile_test_analyzer\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677ABE89-83E3-44A4-8F57-3F8BCC56B4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6633D865-A550-41C0-A5CF-6703FD0D675B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="151">
   <si>
     <t>N° test</t>
   </si>
@@ -108,24 +108,15 @@
     <t>Ouvre une fenêtre de sélection de dossier. Après validation, supprime l'ancienne liste des fichiers et la remplace par la nouvelle.</t>
   </si>
   <si>
-    <t>Ouvre une fenêtre de sélection de fichier. Après validation, le fichier est importé et chaque échantillon dispose de sa propre ligne supplémentaire.</t>
-  </si>
-  <si>
     <t>Cliquer sur bouton d'ajout de fichier.
 Sélection d'un nouveau fichier.
 Cliquer sur valider.</t>
   </si>
   <si>
-    <t>Supprime l'entrée correspondante dans la liste. Vérifier que les autres fichiers s'analysent correctement. Si aucun fichier sélectionner, ne fait rien</t>
-  </si>
-  <si>
     <t>Afficher le menu d'aide</t>
   </si>
   <si>
     <t>Cliquer sur le bouton d'aide.</t>
-  </si>
-  <si>
-    <t>Ouvre la fenêtre d'aide.</t>
   </si>
   <si>
     <t>Changer l'onglet d'affichage des graphiques</t>
@@ -394,9 +385,6 @@
     <t>Importation de fichiers faux</t>
   </si>
   <si>
-    <t>./Data/Erreur.csv</t>
-  </si>
-  <si>
     <t>Le programme analyse le dossier "Data", le fichier posant problème est skippé. Un message d'avertissement apparait pour avertir l'utilisateur.</t>
   </si>
   <si>
@@ -427,10 +415,145 @@
     <t>Cocher la case "Déformation en %". Configurer et analyser le sample. Exporter tous les graphiques individuels</t>
   </si>
   <si>
-    <t>L'axe de "Déformation" dans le graphique "Contrainte - Déformation" doit être en [%], le rp02 passant par la valeur 0.2 %. Si la case est décochée, tout doit être divisé d'un facteur 100 et rp02 doit passer par la valeur 0.002</t>
-  </si>
-  <si>
     <t>Analyse traction avec extensomètre</t>
+  </si>
+  <si>
+    <t>Affichage de la droite élastique</t>
+  </si>
+  <si>
+    <t>Affichages des tables dans les graphiques</t>
+  </si>
+  <si>
+    <t>Cocher la case "Droite limite élastique". Configurer et analyser le sample. Exporter tous les graphiques individuels</t>
+  </si>
+  <si>
+    <t>Cocher la case "Montrer résultats calculés". Configurer et analyser le sample. Exporter les graphiques individuels.</t>
+  </si>
+  <si>
+    <t>Les graphiques doivent avoir la table affichées avec les valeurs max du graphiques. Les noms et unités dépendent du type de graphique et sont adaptés au cas par cas.</t>
+  </si>
+  <si>
+    <t>Forcer l'affichage des valeurs de forces en [kN]</t>
+  </si>
+  <si>
+    <t>Cocher la case "Utilisation des {kN}". Configurer et analyser le sample. Exporter les graphiques individuels.</t>
+  </si>
+  <si>
+    <t>Les graphiques "Forces" doivent avoir l'axe adapté d'un facteur 1000. Les tables doivent aussi avoir la valeur adaptée.</t>
+  </si>
+  <si>
+    <t>Comportement des option d'analyse</t>
+  </si>
+  <si>
+    <t>Changement des chiffres significatifs</t>
+  </si>
+  <si>
+    <t>Passer l'option des chiffres significatifs sur 5. Configurer et analyser le sample. Exporter les graphiques individuels. Ouvrir la fenêtre des variables.</t>
+  </si>
+  <si>
+    <t>Les chiffres significatifs devraient être de 5 partout où cela est possible: Les tables des graphiques exportés; Fenêtre des variables; Fenêtre post-analyse et tableaux exportés (VarWin &amp; PAWin).</t>
+  </si>
+  <si>
+    <t>Changement dedéfinition limite élastique</t>
+  </si>
+  <si>
+    <t>Passer l'option de Définition de limite élastique à 0.5% pour optenir Rp0.5 par la suite. Configurer et analyser le sample. Exporter les graphiques individuels.</t>
+  </si>
+  <si>
+    <t>La définition de Re passe à 0.5%. Les résultats calculés pour Re doivent avoir été adaptés en conséquence. Vérifier sur les graphique "Contrainte - Déformation" que la droite change bien de position.</t>
+  </si>
+  <si>
+    <t>Le programme s'exécute sans erreur et la fenêtre principale s'ouvre. Si un fichier est présent mais n'est pas reconnu comme valide, le programme le skip</t>
+  </si>
+  <si>
+    <t>Le programme s'exécute correctement</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Le programme détecte les fichiers correctement et les listes correctement</t>
+  </si>
+  <si>
+    <t>Le programme détecte les fichiers multiples correctement. Chaque sample est disposé sur une ligne</t>
+  </si>
+  <si>
+    <t>Le programme détecte le problème, skip le fichier et averti l'utilisateur.</t>
+  </si>
+  <si>
+    <t>./Data/Exemple_Erreur_Import_Largeur_Incorrecte.csv</t>
+  </si>
+  <si>
+    <t>Ouvre une fenêtre de sélection de fichier. Après validation, le fichier est importé et chaque échantillon dispose de sa propre ligne supplémentaire. Vérifier pour chaque machine et avec un fichier multisample et un fichier faux.</t>
+  </si>
+  <si>
+    <t>Le programme ajoute correctement les fichiers à la liste et sépare correctement les échantillons</t>
+  </si>
+  <si>
+    <t>Supprime l'entrée correspondante dans la liste. Vérifier que les autres fichiers s'analysent correctement. Si aucun fichier sélectionner, ne fait rien. La liste de fichier est mise à jour correctement et le reste des comportement n'est pas affecté</t>
+  </si>
+  <si>
+    <t>Caution</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Supprime l'entrée correspondante. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Peut affecter l'affichage de la liste de fichier (raison inconnue).</t>
+    </r>
+  </si>
+  <si>
+    <t>La liste est supprimée puis mise à jour avec les fichiers du nouveau répertoire</t>
+  </si>
+  <si>
+    <t>Ouvre la fenêtre d'aide. 3 onglets sont sélectionnables. La navigation entre les onglets change les images d'aide</t>
+  </si>
+  <si>
+    <t>La fenêtre s'ouvre et se ferme correctement. La navigation fonctionne entre les pages d'aide.</t>
+  </si>
+  <si>
+    <t>La navigation entre les pages fonctionne correctement. Les axes sont adaptés en fonction du cas.</t>
+  </si>
+  <si>
+    <t>La fenêtre s'ouvre et fonctionne correctement. Les données affichées correspondent à celles inscrites ou importées.</t>
+  </si>
+  <si>
+    <t>Les graphiques sont exportés correctement. Les options d'exportations fonctionnent aussi et les graphiques sont adaptés en fonction du cas.</t>
+  </si>
+  <si>
+    <t>La fenêtre de configuration fonctionne correctement. Les champs sont sauvegarder et la fenêtre retrouve ses valeurs si on la ferme et rouvre.</t>
+  </si>
+  <si>
+    <t>Le comportement au clique sur les élements de la liste fonctionne correctement. Le fichier sélectionné est en rouge et le grpahique affiché est correcte.</t>
+  </si>
+  <si>
+    <t>Le comportement des onglets de navigation fonctionne correctement et les images sont mises à jour correctement.</t>
+  </si>
+  <si>
+    <t>Les boutons radio fonctionnent correctement. Les images sont mise à jour correctement et les champs aussi.</t>
+  </si>
+  <si>
+    <t>Les menus sont grisés, ce qui est correcte pour la shimadzu</t>
+  </si>
+  <si>
+    <t>Le menu de sélection de l'extenso pour la W+B100kN permet de changer le canal de déplacement. Les graphiques changent correctement</t>
+  </si>
+  <si>
+    <t>Les menus sont grisés, ce qui est correcte pour la W+B 400kN</t>
+  </si>
+  <si>
+    <t>Les valeurs sont sauvegardées correctement. Les valeurs apparaissent à nouveau lors de la femeture + rouverture de la fenêtre de configuration</t>
+  </si>
+  <si>
+    <t>La modification du nom dans la fenêtre de configuration entraine un changement de nom dans l'interface principale ainsi que sur les graphiques (tous, y compris ceux exportés)</t>
   </si>
   <si>
     <t>Configurer l'échantillon comme cela : 
@@ -439,87 +562,106 @@
 Géométrie : Ronde
 D0 = 2
 L0 = 100
-F_Max = 4000
-F_Min = 2000</t>
+F_Max = 1200
+F_Min = 600</t>
   </si>
   <si>
     <t>Résultats Correctes (DataExtractorV10):
-F_Max = 8340 N
-Allong = 18.3 mm (A controler)
-Re = 2010 MPa
+F_Max = 2300 N
+Allong = 5.31 mm
+Re = 719 MPa
+Rm = 732 Mpa
+Defo = 4.57 % 
+E = 82.5 GPa</t>
+  </si>
+  <si>
+    <t>Les noms des graphiques et les légendes sont adaptés en fonction du cas. Les noms utilisés sont correctes</t>
+  </si>
+  <si>
+    <t>Le comportement de l'option "Legende" fonctionne correctement</t>
+  </si>
+  <si>
+    <t>L'axe de "Déformation" dans le graphique "Contrainte - Déformation" doit être en [%], le rp02 passant par la valeur 0.2 %. Si la case est décochée, tout doit être divisé d'un facteur 100 et rp02 doit passer par la valeur 0.002. Les tables doivent être adaptées.</t>
+  </si>
+  <si>
+    <t>Rien ne change. Il n'y a pas de modification dans les graphique. (Pas implémenté ?)</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Le graphique "Contrainte - Déformation" ne doit plus contenir la droite de limite élastique si la case est décochée. La droite est présente si la case est cochée.</t>
+  </si>
+  <si>
+    <t>La droite limite élastique est présente (ou pas) correctement</t>
+  </si>
+  <si>
+    <t>La table sur les graphiques est présente (ou pas) correctement</t>
+  </si>
+  <si>
+    <t>Les graphiques sont adaptés correctement en fonction du cas. Les valeurs sont aussi adaptées.</t>
+  </si>
+  <si>
+    <t>Les chiffres significatifs sont correctement adaptés. Les tables dans les graphiques et fenêtres sont conformes</t>
+  </si>
+  <si>
+    <t>La définition de Re est correcte par rapport à ce qui est défini. Les graphiques ne se mettent à jour qu'après analyse, pas au changement de définition</t>
+  </si>
+  <si>
+    <t>Résultats obtenus:
+F_max = 8340 N
+Allong = 18,6 mm
+Re = 2010 Mpa
 Rm = 2660 Mpa
-Defo = 17.3 % 
-E = 169 GPa</t>
-  </si>
-  <si>
-    <t>Affichage de la droite élastique</t>
-  </si>
-  <si>
-    <t>Le graphique "Contrainte - Déformation" ne doit plus contenir la droite de limite élastique.</t>
-  </si>
-  <si>
-    <t>Affichages des tables dans les graphiques</t>
-  </si>
-  <si>
-    <t>Cocher la case "Droite limite élastique". Configurer et analyser le sample. Exporter tous les graphiques individuels</t>
-  </si>
-  <si>
-    <t>Cocher la case "Montrer résultats calculés". Configurer et analyser le sample. Exporter les graphiques individuels.</t>
-  </si>
-  <si>
-    <t>Les graphiques doivent avoir la table affichées avec les valeurs max du graphiques. Les noms et unités dépendent du type de graphique et sont adaptés au cas par cas.</t>
-  </si>
-  <si>
-    <t>Forcer l'affichage des valeurs de forces en [kN]</t>
-  </si>
-  <si>
-    <t>Cocher la case "Utilisation des {kN}". Configurer et analyser le sample. Exporter les graphiques individuels.</t>
-  </si>
-  <si>
-    <t>Les graphiques "Forces" doivent avoir l'axe adapté d'un facteur 1000. Les tables doivent aussi avoir la valeur adaptée.</t>
-  </si>
-  <si>
-    <t>Comportement des option d'analyse</t>
-  </si>
-  <si>
-    <t>Changement des chiffres significatifs</t>
-  </si>
-  <si>
-    <t>Passer l'option des chiffres significatifs sur 5. Configurer et analyser le sample. Exporter les graphiques individuels. Ouvrir la fenêtre des variables.</t>
-  </si>
-  <si>
-    <t>Les chiffres significatifs devraient être de 5 partout où cela est possible: Les tables des graphiques exportés; Fenêtre des variables; Fenêtre post-analyse et tableaux exportés (VarWin &amp; PAWin).</t>
-  </si>
-  <si>
-    <t>Changement dedéfinition limite élastique</t>
-  </si>
-  <si>
-    <t>Passer l'option de Définition de limite élastique à 0.5% pour optenir Rp0.5 par la suite. Configurer et analyser le sample. Exporter les graphiques individuels.</t>
-  </si>
-  <si>
-    <t>La définition de Re passe à 0.5%. Les résultats calculés pour Re doivent avoir été adaptés en conséquence. Vérifier sur les graphique "Contrainte - Déformation" que la droite change bien de position.</t>
-  </si>
-  <si>
-    <t>Le programme s'exécute sans erreur et la fenêtre principale s'ouvre. Si un fichier est présent mais n'est pas reconnu comme valide, le programme le skip</t>
-  </si>
-  <si>
-    <t>Le programme s'exécute correctement</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Le programme détecte les fichiers correctement et les listes correctement</t>
-  </si>
-  <si>
-    <t>Le programme détecte les fichiers multiples correctement. Chaque sample est disposé sur une ligne</t>
+Defo = 17.3 %
+E = 169 Gpa</t>
+  </si>
+  <si>
+    <t>Résultats obtenus : 
+F_Max = 2300 N
+Allong = 5.3 mm
+Re = 718 Mpa
+Rm = 732 Mpa
+Defo = 4.52 %
+E = 82.6 Gpa</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Résultats obtenus : 
+F_Max = 525 N
+Allong =  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.32 mm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Re = 3040 Mpa
+Rm = 3340 Mpa
+Defo = 0,647 %
+E = 291 Gpa</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -538,6 +680,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -563,7 +711,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -580,6 +728,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -918,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="D28" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -927,7 +1078,7 @@
     <col min="1" max="1" width="9.21875" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" style="6" customWidth="1"/>
     <col min="3" max="3" width="24.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="46.109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="32.6640625" style="1" customWidth="1"/>
@@ -977,13 +1128,13 @@
         <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="H2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1006,10 +1157,10 @@
         <v>11</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="H3" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1032,10 +1183,10 @@
         <v>13</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="H4" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1046,16 +1197,22 @@
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D5" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>86</v>
+      <c r="F5" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H5" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1063,7 +1220,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
@@ -1072,18 +1229,24 @@
         <v>15</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>16</v>
@@ -1092,7 +1255,13 @@
         <v>22</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>27</v>
+        <v>117</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H7" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1100,7 +1269,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>17</v>
@@ -1113,6 +1282,12 @@
       </c>
       <c r="F8" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1120,16 +1295,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>30</v>
+        <v>121</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H9" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -1137,16 +1318,25 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H10" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -1154,19 +1344,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H11" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -1174,59 +1370,77 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H14" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -1234,19 +1448,25 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H15" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1254,379 +1474,481 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D17" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="G17" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G18" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" t="s">
         <v>59</v>
       </c>
-      <c r="D19" t="s">
-        <v>62</v>
-      </c>
       <c r="E19" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="G22" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D23" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="H24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D25" t="s">
-        <v>78</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G27" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H27" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D28" t="s">
         <v>10</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="D29" t="s">
         <v>10</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H29" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D30" t="s">
         <v>10</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D31" t="s">
         <v>10</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H31" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D32" t="s">
         <v>10</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D33" t="s">
         <v>10</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D34" t="s">
         <v>10</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>115</v>
+        <v>107</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H34" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changement résultat test option%
</commit_message>
<xml_diff>
--- a/test/Tensile_test.xlsx
+++ b/test/Tensile_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quentin.raball\Documents\Python\tensile_test_analyzer\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6633D865-A550-41C0-A5CF-6703FD0D675B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5452081-C35D-4355-BCD5-454AF5E58BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="150">
   <si>
     <t>N° test</t>
   </si>
@@ -412,9 +412,6 @@
     <t>Déformation affichée en %</t>
   </si>
   <si>
-    <t>Cocher la case "Déformation en %". Configurer et analyser le sample. Exporter tous les graphiques individuels</t>
-  </si>
-  <si>
     <t>Analyse traction avec extensomètre</t>
   </si>
   <si>
@@ -579,15 +576,6 @@
   </si>
   <si>
     <t>Le comportement de l'option "Legende" fonctionne correctement</t>
-  </si>
-  <si>
-    <t>L'axe de "Déformation" dans le graphique "Contrainte - Déformation" doit être en [%], le rp02 passant par la valeur 0.2 %. Si la case est décochée, tout doit être divisé d'un facteur 100 et rp02 doit passer par la valeur 0.002. Les tables doivent être adaptées.</t>
-  </si>
-  <si>
-    <t>Rien ne change. Il n'y a pas de modification dans les graphique. (Pas implémenté ?)</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
   <si>
     <t>Le graphique "Contrainte - Déformation" ne doit plus contenir la droite de limite élastique si la case est décochée. La droite est présente si la case est cochée.</t>
@@ -655,6 +643,15 @@
 Defo = 0,647 %
 E = 291 Gpa</t>
     </r>
+  </si>
+  <si>
+    <t>Cocher la case "Déformation en %". Configurer et analyser le sample. Exporter tous les graphiques individuels et exporter le graphique du résumé.</t>
+  </si>
+  <si>
+    <t>L'axe de "Déformation" dans le graphique "Contrainte - Déformation" doit être en [%], le rp02 passant par la valeur 0.2 %. Si la case est décochée, tout doit être divisé d'un facteur 100 et rp02 doit passer par la valeur 0.002. Les valeurs et unités dans les tables doivent être adaptées.</t>
+  </si>
+  <si>
+    <t>L'axe est adapté. Les valeurs du graphique sont adaptées. Les valeurs et unités des tables sont adaptés et fonctionnent correctement.</t>
   </si>
 </sst>
 </file>
@@ -1069,8 +1066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D28" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1128,13 +1125,13 @@
         <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="H2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1157,10 +1154,10 @@
         <v>11</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1183,10 +1180,10 @@
         <v>13</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1200,7 +1197,7 @@
         <v>81</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>21</v>
@@ -1209,10 +1206,10 @@
         <v>82</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1232,13 +1229,13 @@
         <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="H6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -1255,13 +1252,13 @@
         <v>22</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H7" t="s">
         <v>117</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="H7" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1284,10 +1281,10 @@
         <v>24</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1304,13 +1301,13 @@
         <v>27</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="H9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -1333,10 +1330,10 @@
         <v>42</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -1359,10 +1356,10 @@
         <v>32</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -1385,10 +1382,10 @@
         <v>35</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -1411,10 +1408,10 @@
         <v>39</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -1437,10 +1434,10 @@
         <v>43</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -1463,10 +1460,10 @@
         <v>47</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1489,10 +1486,10 @@
         <v>50</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1515,10 +1512,10 @@
         <v>57</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -1541,10 +1538,10 @@
         <v>58</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1567,10 +1564,10 @@
         <v>60</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -1593,10 +1590,10 @@
         <v>63</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -1619,10 +1616,10 @@
         <v>66</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1645,10 +1642,10 @@
         <v>70</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
@@ -1659,22 +1656,22 @@
         <v>67</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D23" t="s">
         <v>53</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F23" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="F23" s="7" t="s">
-        <v>136</v>
-      </c>
       <c r="G23" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
@@ -1697,10 +1694,10 @@
         <v>72</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
@@ -1763,10 +1760,10 @@
         <v>89</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1789,13 +1786,13 @@
         <v>88</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1809,16 +1806,16 @@
         <v>10</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>91</v>
+        <v>147</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="H29" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1829,22 +1826,22 @@
         <v>86</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D30" t="s">
         <v>10</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -1855,22 +1852,22 @@
         <v>86</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D31" t="s">
         <v>10</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="G31" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1881,22 +1878,22 @@
         <v>86</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D32" t="s">
         <v>10</v>
       </c>
       <c r="E32" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="G32" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="H32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -1904,25 +1901,25 @@
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="D33" t="s">
         <v>10</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="G33" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="H33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -1930,25 +1927,25 @@
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D34" t="s">
         <v>10</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="G34" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>